<commit_message>
added comments to the code
</commit_message>
<xml_diff>
--- a/MATLAB/results_analytical.xlsx
+++ b/MATLAB/results_analytical.xlsx
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD4F1E0-155A-4FE3-87CC-4881CBE012D3}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="A3" sqref="A3:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,6 +493,118 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>0.04</v>
+      </c>
+      <c r="K2">
+        <v>0.03</v>
+      </c>
+      <c r="L2">
+        <v>0.02</v>
+      </c>
+      <c r="M2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N2">
+        <v>200</v>
+      </c>
+      <c r="O2">
+        <v>300</v>
+      </c>
+      <c r="P2">
+        <v>600</v>
+      </c>
+      <c r="Q2">
+        <v>0.2822010582010584</v>
+      </c>
+      <c r="R2">
+        <v>0.75000000000000011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5.6</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>0.04</v>
+      </c>
+      <c r="K3">
+        <v>0.03</v>
+      </c>
+      <c r="L3">
+        <v>0.02</v>
+      </c>
+      <c r="M3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N3">
+        <v>200</v>
+      </c>
+      <c r="O3">
+        <v>300</v>
+      </c>
+      <c r="P3">
+        <v>600</v>
+      </c>
+      <c r="Q3">
+        <v>0.18195978835978824</v>
+      </c>
+      <c r="R3">
+        <v>0.75675675675675691</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
disable save button while saving data
</commit_message>
<xml_diff>
--- a/MATLAB/results_analytical.xlsx
+++ b/MATLAB/results_analytical.xlsx
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD4F1E0-155A-4FE3-87CC-4881CBE012D3}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:R3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,118 +493,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5.4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>0.04</v>
-      </c>
-      <c r="K2">
-        <v>0.03</v>
-      </c>
-      <c r="L2">
-        <v>0.02</v>
-      </c>
-      <c r="M2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N2">
-        <v>200</v>
-      </c>
-      <c r="O2">
-        <v>300</v>
-      </c>
-      <c r="P2">
-        <v>600</v>
-      </c>
-      <c r="Q2">
-        <v>0.2822010582010584</v>
-      </c>
-      <c r="R2">
-        <v>0.75000000000000011</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5.6</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>0.04</v>
-      </c>
-      <c r="K3">
-        <v>0.03</v>
-      </c>
-      <c r="L3">
-        <v>0.02</v>
-      </c>
-      <c r="M3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N3">
-        <v>200</v>
-      </c>
-      <c r="O3">
-        <v>300</v>
-      </c>
-      <c r="P3">
-        <v>600</v>
-      </c>
-      <c r="Q3">
-        <v>0.18195978835978824</v>
-      </c>
-      <c r="R3">
-        <v>0.75675675675675691</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed formulae to M/D/1 and added go nogo indication
</commit_message>
<xml_diff>
--- a/MATLAB/results_analytical.xlsx
+++ b/MATLAB/results_analytical.xlsx
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD4F1E0-155A-4FE3-87CC-4881CBE012D3}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A4" sqref="A4:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,6 +493,174 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>0.04</v>
+      </c>
+      <c r="K2">
+        <v>0.03</v>
+      </c>
+      <c r="L2">
+        <v>0.02</v>
+      </c>
+      <c r="M2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N2">
+        <v>200</v>
+      </c>
+      <c r="O2">
+        <v>300</v>
+      </c>
+      <c r="P2">
+        <v>600</v>
+      </c>
+      <c r="Q2">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="R2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5.8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>0.04</v>
+      </c>
+      <c r="K3">
+        <v>0.03</v>
+      </c>
+      <c r="L3">
+        <v>0.02</v>
+      </c>
+      <c r="M3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N3">
+        <v>200</v>
+      </c>
+      <c r="O3">
+        <v>300</v>
+      </c>
+      <c r="P3">
+        <v>600</v>
+      </c>
+      <c r="Q3">
+        <v>0.214</v>
+      </c>
+      <c r="R3">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5.8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>0.04</v>
+      </c>
+      <c r="K4">
+        <v>0.03</v>
+      </c>
+      <c r="L4">
+        <v>0.02</v>
+      </c>
+      <c r="M4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N4">
+        <v>200</v>
+      </c>
+      <c r="O4">
+        <v>300</v>
+      </c>
+      <c r="P4">
+        <v>600</v>
+      </c>
+      <c r="Q4">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="R4">
+        <v>0.76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed default UI values
</commit_message>
<xml_diff>
--- a/MATLAB/results_analytical.xlsx
+++ b/MATLAB/results_analytical.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samvrit\Box Sync\ENSE 623 - System Verification\Project\MATLAB\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{94A00B17-13C9-40F2-8B6B-1E705B80A754}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,18 +416,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD4F1E0-155A-4FE3-87CC-4881CBE012D3}">
-  <dimension ref="A1:R4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:R4"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,174 +488,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5.4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>0.04</v>
-      </c>
-      <c r="K2">
-        <v>0.03</v>
-      </c>
-      <c r="L2">
-        <v>0.02</v>
-      </c>
-      <c r="M2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N2">
-        <v>200</v>
-      </c>
-      <c r="O2">
-        <v>300</v>
-      </c>
-      <c r="P2">
-        <v>600</v>
-      </c>
-      <c r="Q2">
-        <v>0.28199999999999997</v>
-      </c>
-      <c r="R2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5.8</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>0.04</v>
-      </c>
-      <c r="K3">
-        <v>0.03</v>
-      </c>
-      <c r="L3">
-        <v>0.02</v>
-      </c>
-      <c r="M3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N3">
-        <v>200</v>
-      </c>
-      <c r="O3">
-        <v>300</v>
-      </c>
-      <c r="P3">
-        <v>600</v>
-      </c>
-      <c r="Q3">
-        <v>0.214</v>
-      </c>
-      <c r="R3">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5.8</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>0.04</v>
-      </c>
-      <c r="K4">
-        <v>0.03</v>
-      </c>
-      <c r="L4">
-        <v>0.02</v>
-      </c>
-      <c r="M4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N4">
-        <v>200</v>
-      </c>
-      <c r="O4">
-        <v>300</v>
-      </c>
-      <c r="P4">
-        <v>600</v>
-      </c>
-      <c r="Q4">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="R4">
-        <v>0.76</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added test case table and results
</commit_message>
<xml_diff>
--- a/MATLAB/results_analytical.xlsx
+++ b/MATLAB/results_analytical.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -416,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,960 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.04</v>
+      </c>
+      <c r="K2">
+        <v>0.04</v>
+      </c>
+      <c r="L2">
+        <v>0.04</v>
+      </c>
+      <c r="M2">
+        <v>0.04</v>
+      </c>
+      <c r="N2">
+        <v>50</v>
+      </c>
+      <c r="O2">
+        <v>200</v>
+      </c>
+      <c r="P2">
+        <v>550</v>
+      </c>
+      <c r="Q2">
+        <v>-4503599627370.4561</v>
+      </c>
+      <c r="R2">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.04</v>
+      </c>
+      <c r="K3">
+        <v>0.04</v>
+      </c>
+      <c r="L3">
+        <v>0.04</v>
+      </c>
+      <c r="M3">
+        <v>0.04</v>
+      </c>
+      <c r="N3">
+        <v>50</v>
+      </c>
+      <c r="O3">
+        <v>200</v>
+      </c>
+      <c r="P3">
+        <v>650</v>
+      </c>
+      <c r="Q3">
+        <v>-4503599627370.457</v>
+      </c>
+      <c r="R3">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.04</v>
+      </c>
+      <c r="K4">
+        <v>0.04</v>
+      </c>
+      <c r="L4">
+        <v>0.04</v>
+      </c>
+      <c r="M4">
+        <v>0.04</v>
+      </c>
+      <c r="N4">
+        <v>50</v>
+      </c>
+      <c r="O4">
+        <v>400</v>
+      </c>
+      <c r="P4">
+        <v>550</v>
+      </c>
+      <c r="Q4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="R4">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.04</v>
+      </c>
+      <c r="K5">
+        <v>0.04</v>
+      </c>
+      <c r="L5">
+        <v>0.04</v>
+      </c>
+      <c r="M5">
+        <v>0.04</v>
+      </c>
+      <c r="N5">
+        <v>50</v>
+      </c>
+      <c r="O5">
+        <v>400</v>
+      </c>
+      <c r="P5">
+        <v>650</v>
+      </c>
+      <c r="Q5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="R5">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0.04</v>
+      </c>
+      <c r="K6">
+        <v>0.04</v>
+      </c>
+      <c r="L6">
+        <v>0.04</v>
+      </c>
+      <c r="M6">
+        <v>0.04</v>
+      </c>
+      <c r="N6">
+        <v>150</v>
+      </c>
+      <c r="O6">
+        <v>200</v>
+      </c>
+      <c r="P6">
+        <v>550</v>
+      </c>
+      <c r="Q6">
+        <v>-4503599627370.4502</v>
+      </c>
+      <c r="R6">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.04</v>
+      </c>
+      <c r="K7">
+        <v>0.04</v>
+      </c>
+      <c r="L7">
+        <v>0.04</v>
+      </c>
+      <c r="M7">
+        <v>0.04</v>
+      </c>
+      <c r="N7">
+        <v>150</v>
+      </c>
+      <c r="O7">
+        <v>200</v>
+      </c>
+      <c r="P7">
+        <v>650</v>
+      </c>
+      <c r="Q7">
+        <v>-4503599627370.4512</v>
+      </c>
+      <c r="R7">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0.04</v>
+      </c>
+      <c r="K8">
+        <v>0.04</v>
+      </c>
+      <c r="L8">
+        <v>0.04</v>
+      </c>
+      <c r="M8">
+        <v>0.04</v>
+      </c>
+      <c r="N8">
+        <v>150</v>
+      </c>
+      <c r="O8">
+        <v>400</v>
+      </c>
+      <c r="P8">
+        <v>550</v>
+      </c>
+      <c r="Q8">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="R8">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0.04</v>
+      </c>
+      <c r="K9">
+        <v>0.04</v>
+      </c>
+      <c r="L9">
+        <v>0.04</v>
+      </c>
+      <c r="M9">
+        <v>0.04</v>
+      </c>
+      <c r="N9">
+        <v>150</v>
+      </c>
+      <c r="O9">
+        <v>400</v>
+      </c>
+      <c r="P9">
+        <v>650</v>
+      </c>
+      <c r="Q9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="R9">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0.02</v>
+      </c>
+      <c r="K10">
+        <v>0.02</v>
+      </c>
+      <c r="L10">
+        <v>0.02</v>
+      </c>
+      <c r="M10">
+        <v>0.02</v>
+      </c>
+      <c r="N10">
+        <v>50</v>
+      </c>
+      <c r="O10">
+        <v>200</v>
+      </c>
+      <c r="P10">
+        <v>550</v>
+      </c>
+      <c r="Q10">
+        <v>65535</v>
+      </c>
+      <c r="R10">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0.02</v>
+      </c>
+      <c r="K11">
+        <v>0.02</v>
+      </c>
+      <c r="L11">
+        <v>0.02</v>
+      </c>
+      <c r="M11">
+        <v>0.02</v>
+      </c>
+      <c r="N11">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <v>200</v>
+      </c>
+      <c r="P11">
+        <v>650</v>
+      </c>
+      <c r="Q11">
+        <v>65535</v>
+      </c>
+      <c r="R11">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0.02</v>
+      </c>
+      <c r="K12">
+        <v>0.02</v>
+      </c>
+      <c r="L12">
+        <v>0.02</v>
+      </c>
+      <c r="M12">
+        <v>0.02</v>
+      </c>
+      <c r="N12">
+        <v>50</v>
+      </c>
+      <c r="O12">
+        <v>400</v>
+      </c>
+      <c r="P12">
+        <v>550</v>
+      </c>
+      <c r="Q12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="R12">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0.02</v>
+      </c>
+      <c r="K13">
+        <v>0.02</v>
+      </c>
+      <c r="L13">
+        <v>0.02</v>
+      </c>
+      <c r="M13">
+        <v>0.02</v>
+      </c>
+      <c r="N13">
+        <v>50</v>
+      </c>
+      <c r="O13">
+        <v>400</v>
+      </c>
+      <c r="P13">
+        <v>650</v>
+      </c>
+      <c r="Q13">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="R13">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0.02</v>
+      </c>
+      <c r="K14">
+        <v>0.02</v>
+      </c>
+      <c r="L14">
+        <v>0.02</v>
+      </c>
+      <c r="M14">
+        <v>0.02</v>
+      </c>
+      <c r="N14">
+        <v>150</v>
+      </c>
+      <c r="O14">
+        <v>200</v>
+      </c>
+      <c r="P14">
+        <v>550</v>
+      </c>
+      <c r="Q14">
+        <v>65535</v>
+      </c>
+      <c r="R14">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0.02</v>
+      </c>
+      <c r="K15">
+        <v>0.02</v>
+      </c>
+      <c r="L15">
+        <v>0.02</v>
+      </c>
+      <c r="M15">
+        <v>0.02</v>
+      </c>
+      <c r="N15">
+        <v>150</v>
+      </c>
+      <c r="O15">
+        <v>200</v>
+      </c>
+      <c r="P15">
+        <v>650</v>
+      </c>
+      <c r="Q15">
+        <v>65535</v>
+      </c>
+      <c r="R15">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0.02</v>
+      </c>
+      <c r="K16">
+        <v>0.02</v>
+      </c>
+      <c r="L16">
+        <v>0.02</v>
+      </c>
+      <c r="M16">
+        <v>0.02</v>
+      </c>
+      <c r="N16">
+        <v>150</v>
+      </c>
+      <c r="O16">
+        <v>400</v>
+      </c>
+      <c r="P16">
+        <v>550</v>
+      </c>
+      <c r="Q16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="R16">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0.02</v>
+      </c>
+      <c r="K17">
+        <v>0.02</v>
+      </c>
+      <c r="L17">
+        <v>0.02</v>
+      </c>
+      <c r="M17">
+        <v>0.02</v>
+      </c>
+      <c r="N17">
+        <v>150</v>
+      </c>
+      <c r="O17">
+        <v>400</v>
+      </c>
+      <c r="P17">
+        <v>650</v>
+      </c>
+      <c r="Q17">
+        <v>2.4E-2</v>
+      </c>
+      <c r="R17">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0.03</v>
+      </c>
+      <c r="K18">
+        <v>0.03</v>
+      </c>
+      <c r="L18">
+        <v>0.03</v>
+      </c>
+      <c r="M18">
+        <v>0.03</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18">
+        <v>300</v>
+      </c>
+      <c r="P18">
+        <v>600</v>
+      </c>
+      <c r="Q18">
+        <v>0.06</v>
+      </c>
+      <c r="R18">
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made idle time = 1-rho
</commit_message>
<xml_diff>
--- a/MATLAB/results_analytical.xlsx
+++ b/MATLAB/results_analytical.xlsx
@@ -416,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -427,7 +427,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
         <v>-4503599627370.4561</v>
       </c>
       <c r="R2">
-        <v>1.1100000000000001</v>
+        <v>-0.1100000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>-4503599627370.457</v>
       </c>
       <c r="R3">
-        <v>1.1100000000000001</v>
+        <v>-0.1100000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="R4">
-        <v>0.55000000000000004</v>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="R5">
-        <v>0.55000000000000004</v>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -765,7 +765,7 @@
         <v>-4503599627370.4502</v>
       </c>
       <c r="R6">
-        <v>1.1100000000000001</v>
+        <v>-0.1100000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -821,7 +821,7 @@
         <v>-4503599627370.4512</v>
       </c>
       <c r="R7">
-        <v>1.1100000000000001</v>
+        <v>-0.1100000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="R8">
-        <v>0.55000000000000004</v>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="R9">
-        <v>0.55000000000000004</v>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -989,7 +989,7 @@
         <v>65535</v>
       </c>
       <c r="R10">
-        <v>1.33</v>
+        <v>-0.33000000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1045,7 +1045,7 @@
         <v>65535</v>
       </c>
       <c r="R11">
-        <v>1.33</v>
+        <v>-0.33000000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1101,7 +1101,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="R12">
-        <v>0.66</v>
+        <v>0.33999999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1157,7 +1157,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="R13">
-        <v>0.66</v>
+        <v>0.33999999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
         <v>65535</v>
       </c>
       <c r="R14">
-        <v>1.33</v>
+        <v>-0.33000000000000007</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1269,7 +1269,7 @@
         <v>65535</v>
       </c>
       <c r="R15">
-        <v>1.33</v>
+        <v>-0.33000000000000007</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1325,7 +1325,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="R16">
-        <v>0.66</v>
+        <v>0.33999999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1381,7 +1381,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="R17">
-        <v>0.66</v>
+        <v>0.33999999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
         <v>0.06</v>
       </c>
       <c r="R18">
-        <v>0.8</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed result for reference test case
</commit_message>
<xml_diff>
--- a/MATLAB/results_analytical.xlsx
+++ b/MATLAB/results_analytical.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samvrit\Box Sync\ENSE 623 - System Verification\Project\MATLAB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,18 +421,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,16 +1418,16 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="K18">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="L18">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M18">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="N18">
         <v>100</v>
@@ -1434,10 +1439,10 @@
         <v>600</v>
       </c>
       <c r="Q18">
-        <v>3.4000000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="R18">
-        <v>0.12</v>
+        <v>0.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added testing program and updated results
</commit_message>
<xml_diff>
--- a/MATLAB/results_analytical.xlsx
+++ b/MATLAB/results_analytical.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Speed</t>
   </si>
@@ -432,7 +433,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,14 +1440,929 @@
         <v>600</v>
       </c>
       <c r="Q18">
-        <v>3.5000000000000003E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="R18">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587952D4-0879-494B-BD8C-DA21DF6ECF12}">
+  <dimension ref="A1:P18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.02</v>
+      </c>
+      <c r="K2">
+        <v>0.02</v>
+      </c>
+      <c r="L2">
+        <v>0.02</v>
+      </c>
+      <c r="M2">
+        <v>0.02</v>
+      </c>
+      <c r="N2">
+        <v>50</v>
+      </c>
+      <c r="O2">
+        <v>200</v>
+      </c>
+      <c r="P2">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.02</v>
+      </c>
+      <c r="K3">
+        <v>0.02</v>
+      </c>
+      <c r="L3">
+        <v>0.02</v>
+      </c>
+      <c r="M3">
+        <v>0.02</v>
+      </c>
+      <c r="N3">
+        <v>50</v>
+      </c>
+      <c r="O3">
+        <v>200</v>
+      </c>
+      <c r="P3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.02</v>
+      </c>
+      <c r="K4">
+        <v>0.02</v>
+      </c>
+      <c r="L4">
+        <v>0.02</v>
+      </c>
+      <c r="M4">
+        <v>0.02</v>
+      </c>
+      <c r="N4">
+        <v>50</v>
+      </c>
+      <c r="O4">
+        <v>400</v>
+      </c>
+      <c r="P4">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.02</v>
+      </c>
+      <c r="K5">
+        <v>0.02</v>
+      </c>
+      <c r="L5">
+        <v>0.02</v>
+      </c>
+      <c r="M5">
+        <v>0.02</v>
+      </c>
+      <c r="N5">
+        <v>50</v>
+      </c>
+      <c r="O5">
+        <v>400</v>
+      </c>
+      <c r="P5">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0.02</v>
+      </c>
+      <c r="K6">
+        <v>0.02</v>
+      </c>
+      <c r="L6">
+        <v>0.02</v>
+      </c>
+      <c r="M6">
+        <v>0.02</v>
+      </c>
+      <c r="N6">
+        <v>150</v>
+      </c>
+      <c r="O6">
+        <v>200</v>
+      </c>
+      <c r="P6">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.02</v>
+      </c>
+      <c r="K7">
+        <v>0.02</v>
+      </c>
+      <c r="L7">
+        <v>0.02</v>
+      </c>
+      <c r="M7">
+        <v>0.02</v>
+      </c>
+      <c r="N7">
+        <v>150</v>
+      </c>
+      <c r="O7">
+        <v>200</v>
+      </c>
+      <c r="P7">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0.02</v>
+      </c>
+      <c r="K8">
+        <v>0.02</v>
+      </c>
+      <c r="L8">
+        <v>0.02</v>
+      </c>
+      <c r="M8">
+        <v>0.02</v>
+      </c>
+      <c r="N8">
+        <v>150</v>
+      </c>
+      <c r="O8">
+        <v>400</v>
+      </c>
+      <c r="P8">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0.02</v>
+      </c>
+      <c r="K9">
+        <v>0.02</v>
+      </c>
+      <c r="L9">
+        <v>0.02</v>
+      </c>
+      <c r="M9">
+        <v>0.02</v>
+      </c>
+      <c r="N9">
+        <v>150</v>
+      </c>
+      <c r="O9">
+        <v>400</v>
+      </c>
+      <c r="P9">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0.04</v>
+      </c>
+      <c r="K10">
+        <v>0.04</v>
+      </c>
+      <c r="L10">
+        <v>0.04</v>
+      </c>
+      <c r="M10">
+        <v>0.04</v>
+      </c>
+      <c r="N10">
+        <v>50</v>
+      </c>
+      <c r="O10">
+        <v>200</v>
+      </c>
+      <c r="P10">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0.04</v>
+      </c>
+      <c r="K11">
+        <v>0.04</v>
+      </c>
+      <c r="L11">
+        <v>0.04</v>
+      </c>
+      <c r="M11">
+        <v>0.04</v>
+      </c>
+      <c r="N11">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <v>200</v>
+      </c>
+      <c r="P11">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0.04</v>
+      </c>
+      <c r="K12">
+        <v>0.04</v>
+      </c>
+      <c r="L12">
+        <v>0.04</v>
+      </c>
+      <c r="M12">
+        <v>0.04</v>
+      </c>
+      <c r="N12">
+        <v>50</v>
+      </c>
+      <c r="O12">
+        <v>400</v>
+      </c>
+      <c r="P12">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0.04</v>
+      </c>
+      <c r="K13">
+        <v>0.04</v>
+      </c>
+      <c r="L13">
+        <v>0.04</v>
+      </c>
+      <c r="M13">
+        <v>0.04</v>
+      </c>
+      <c r="N13">
+        <v>50</v>
+      </c>
+      <c r="O13">
+        <v>400</v>
+      </c>
+      <c r="P13">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0.04</v>
+      </c>
+      <c r="K14">
+        <v>0.04</v>
+      </c>
+      <c r="L14">
+        <v>0.04</v>
+      </c>
+      <c r="M14">
+        <v>0.04</v>
+      </c>
+      <c r="N14">
+        <v>150</v>
+      </c>
+      <c r="O14">
+        <v>200</v>
+      </c>
+      <c r="P14">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0.04</v>
+      </c>
+      <c r="K15">
+        <v>0.04</v>
+      </c>
+      <c r="L15">
+        <v>0.04</v>
+      </c>
+      <c r="M15">
+        <v>0.04</v>
+      </c>
+      <c r="N15">
+        <v>150</v>
+      </c>
+      <c r="O15">
+        <v>200</v>
+      </c>
+      <c r="P15">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0.04</v>
+      </c>
+      <c r="K16">
+        <v>0.04</v>
+      </c>
+      <c r="L16">
+        <v>0.04</v>
+      </c>
+      <c r="M16">
+        <v>0.04</v>
+      </c>
+      <c r="N16">
+        <v>150</v>
+      </c>
+      <c r="O16">
+        <v>400</v>
+      </c>
+      <c r="P16">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0.04</v>
+      </c>
+      <c r="K17">
+        <v>0.04</v>
+      </c>
+      <c r="L17">
+        <v>0.04</v>
+      </c>
+      <c r="M17">
+        <v>0.04</v>
+      </c>
+      <c r="N17">
+        <v>150</v>
+      </c>
+      <c r="O17">
+        <v>400</v>
+      </c>
+      <c r="P17">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0.03</v>
+      </c>
+      <c r="K18">
+        <v>0.03</v>
+      </c>
+      <c r="L18">
+        <v>0.03</v>
+      </c>
+      <c r="M18">
+        <v>0.03</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18">
+        <v>300</v>
+      </c>
+      <c r="P18">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed analytical-to-montecarlo switching issue and added file to automate montecarlo test
</commit_message>
<xml_diff>
--- a/MATLAB/results_analytical.xlsx
+++ b/MATLAB/results_analytical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>550</v>
       </c>
       <c r="Q2">
-        <v>2.7E-2</v>
+        <v>2.6653264600378528E-2</v>
       </c>
       <c r="R2">
         <v>0.75</v>
@@ -600,7 +600,7 @@
         <v>650</v>
       </c>
       <c r="Q3">
-        <v>2.5999999999999999E-2</v>
+        <v>2.6319931267045193E-2</v>
       </c>
       <c r="R3">
         <v>0.75</v>
@@ -656,10 +656,10 @@
         <v>550</v>
       </c>
       <c r="Q4">
-        <v>2.3E-2</v>
+        <v>2.2843740790854716E-2</v>
       </c>
       <c r="R4">
-        <v>0.88</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -712,10 +712,10 @@
         <v>650</v>
       </c>
       <c r="Q5">
-        <v>2.3E-2</v>
+        <v>2.2510407457521382E-2</v>
       </c>
       <c r="R5">
-        <v>0.88</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -768,7 +768,7 @@
         <v>550</v>
       </c>
       <c r="Q6">
-        <v>5.2999999999999999E-2</v>
+        <v>5.3365157134374536E-2</v>
       </c>
       <c r="R6">
         <v>0.25</v>
@@ -824,7 +824,7 @@
         <v>650</v>
       </c>
       <c r="Q7">
-        <v>5.2999999999999999E-2</v>
+        <v>5.2865157134374535E-2</v>
       </c>
       <c r="R7">
         <v>0.25</v>
@@ -880,10 +880,10 @@
         <v>550</v>
       </c>
       <c r="Q8">
-        <v>3.6999999999999998E-2</v>
+        <v>3.7365157134374535E-2</v>
       </c>
       <c r="R8">
-        <v>0.63</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -936,10 +936,10 @@
         <v>650</v>
       </c>
       <c r="Q9">
-        <v>3.6999999999999998E-2</v>
+        <v>3.6865157134374535E-2</v>
       </c>
       <c r="R9">
-        <v>0.63</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -992,7 +992,7 @@
         <v>550</v>
       </c>
       <c r="Q10">
-        <v>2.3E-2</v>
+        <v>2.3345663665162518E-2</v>
       </c>
       <c r="R10">
         <v>0.75</v>
@@ -1048,7 +1048,7 @@
         <v>650</v>
       </c>
       <c r="Q11">
-        <v>2.3E-2</v>
+        <v>2.3012330331829183E-2</v>
       </c>
       <c r="R11">
         <v>0.75</v>
@@ -1104,10 +1104,10 @@
         <v>550</v>
       </c>
       <c r="Q12">
-        <v>0.02</v>
+        <v>1.9536139855638707E-2</v>
       </c>
       <c r="R12">
-        <v>0.88</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1160,10 +1160,10 @@
         <v>650</v>
       </c>
       <c r="Q13">
-        <v>1.9E-2</v>
+        <v>1.9202806522305372E-2</v>
       </c>
       <c r="R13">
-        <v>0.88</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1216,7 +1216,7 @@
         <v>550</v>
       </c>
       <c r="Q14">
-        <v>4.2999999999999997E-2</v>
+        <v>4.3468070932104357E-2</v>
       </c>
       <c r="R14">
         <v>0.25</v>
@@ -1272,7 +1272,7 @@
         <v>650</v>
       </c>
       <c r="Q15">
-        <v>4.2999999999999997E-2</v>
+        <v>4.2968070932104356E-2</v>
       </c>
       <c r="R15">
         <v>0.25</v>
@@ -1328,10 +1328,10 @@
         <v>550</v>
       </c>
       <c r="Q16">
-        <v>2.7E-2</v>
+        <v>2.746807093210436E-2</v>
       </c>
       <c r="R16">
-        <v>0.63</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1384,10 +1384,10 @@
         <v>650</v>
       </c>
       <c r="Q17">
-        <v>2.7E-2</v>
+        <v>2.6968070932104363E-2</v>
       </c>
       <c r="R17">
-        <v>0.63</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1440,10 +1440,10 @@
         <v>600</v>
       </c>
       <c r="Q18">
-        <v>2.5999999999999999E-2</v>
+        <v>2.6193317254338253E-2</v>
       </c>
       <c r="R18">
-        <v>0.67</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
   </sheetData>
@@ -1456,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587952D4-0879-494B-BD8C-DA21DF6ECF12}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>